<commit_message>
Vaccancy is in progress
IT Ad made and posted in fb groups
</commit_message>
<xml_diff>
--- a/Offline/TeacherRecruitment/FaceBookAdForTeacherRecruitments/FacultyContactDetails.xlsx
+++ b/Offline/TeacherRecruitment/FaceBookAdForTeacherRecruitments/FacultyContactDetails.xlsx
@@ -8,26 +8,36 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Anodiam\Docs\Offline\TeacherRecruitment\FaceBookAdForTeacherRecruitments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4835F7B4-5145-4C28-8C47-CFD6DEA3DA15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C96B07BE-4E94-4607-A04E-AC7D30F7CA9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Faculty Contact Details" sheetId="1" r:id="rId1"/>
-    <sheet name="Faculty Required" sheetId="2" r:id="rId2"/>
-    <sheet name="Loreto-Email-Id" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId2"/>
+    <sheet name="Faculty Required" sheetId="2" r:id="rId3"/>
+    <sheet name="Loreto-Email-Id" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="77">
   <si>
     <t>SlNo</t>
   </si>
@@ -180,13 +190,91 @@
   </si>
   <si>
     <t>IT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ankita Mukherjee </t>
+  </si>
+  <si>
+    <t>Humanities</t>
+  </si>
+  <si>
+    <t>80173 89304</t>
+  </si>
+  <si>
+    <t>Facebook</t>
+  </si>
+  <si>
+    <t>Indrani Banerjee</t>
+  </si>
+  <si>
+    <t>84203 71183</t>
+  </si>
+  <si>
+    <t>MS Office</t>
+  </si>
+  <si>
+    <t>Advanced Excel (VBA)</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>C++</t>
+  </si>
+  <si>
+    <t>HTML, CSS, JavaScript</t>
+  </si>
+  <si>
+    <t>Java</t>
+  </si>
+  <si>
+    <t>Advanced Java</t>
+  </si>
+  <si>
+    <t>.Net (C#, VB.Net)</t>
+  </si>
+  <si>
+    <t>Advanced .Net</t>
+  </si>
+  <si>
+    <t>React, MUI</t>
+  </si>
+  <si>
+    <t>React Native</t>
+  </si>
+  <si>
+    <t>PHP, Wordpress</t>
+  </si>
+  <si>
+    <t>MySQL</t>
+  </si>
+  <si>
+    <t>SQL Server</t>
+  </si>
+  <si>
+    <t>Oracle</t>
+  </si>
+  <si>
+    <t>Firebase</t>
+  </si>
+  <si>
+    <t>Tally</t>
+  </si>
+  <si>
+    <t>Prince2</t>
+  </si>
+  <si>
+    <t>Agile Scrum</t>
+  </si>
+  <si>
+    <t>She will come at 2nd August 2023 at 5 PM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -219,8 +307,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Oxygen"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -233,8 +326,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -242,12 +341,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -267,6 +381,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -549,10 +667,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -740,6 +858,49 @@
         <v>29</v>
       </c>
     </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="4">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1">
+        <v>45135</v>
+      </c>
+      <c r="C9" t="s">
+        <v>51</v>
+      </c>
+      <c r="D9" t="s">
+        <v>52</v>
+      </c>
+      <c r="E9" t="s">
+        <v>53</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="4">
+        <v>8</v>
+      </c>
+      <c r="B10" s="1">
+        <v>45135</v>
+      </c>
+      <c r="C10" t="s">
+        <v>55</v>
+      </c>
+      <c r="D10" t="s">
+        <v>52</v>
+      </c>
+      <c r="E10" t="s">
+        <v>56</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="H10" t="s">
+        <v>76</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -747,10 +908,123 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D85896B1-649E-444D-B0F4-B18948BE8050}">
+  <dimension ref="E2:E20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="5" max="5" width="27.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E2" s="13" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E3" s="13" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E4" s="13" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E5" s="13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E6" s="13" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E7" s="13" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E8" s="13" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E9" s="13" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="10" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E10" s="13" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="11" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E11" s="13" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="12" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E12" s="13" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="13" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E13" s="13" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="14" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E14" s="13" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E15" s="13" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="16" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E16" s="13" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="17" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E17" s="13" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="18" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E18" s="13" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="19" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E19" s="13" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="20" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E20" s="13" t="s">
+        <v>75</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48EAD798-0DF0-4EE2-934F-0A48BED80FA1}">
   <dimension ref="C2:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
@@ -856,7 +1130,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61E91BA0-385B-4F2E-9F21-1D4601101643}">
   <dimension ref="D2"/>
   <sheetViews>

</xml_diff>